<commit_message>
add chart class, other changes & demo
</commit_message>
<xml_diff>
--- a/support/token_pairs.xlsx
+++ b/support/token_pairs.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="20490" windowHeight="7635"/>
+    <workbookView windowWidth="19200" windowHeight="6915"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="43">
   <si>
     <t>blockchain</t>
   </si>
@@ -117,13 +117,34 @@
     <t>0xA1077a294dDE1B09bB078844df40758a5D0f9a27</t>
   </si>
   <si>
+    <t>0xE56043671df55dE5CDf8459710433C10324DE0aE</t>
+  </si>
+  <si>
+    <t>https://dexscreener.com/pulsechain/0xE56043671df55dE5CDf8459710433C10324DE0aE</t>
+  </si>
+  <si>
+    <t>0x146e1f1e060e5b5016db0d118d2c5a11a240ae32</t>
+  </si>
+  <si>
+    <t>https://dexscreener.com/pulsechain/0x146e1f1e060e5b5016db0d118d2c5a11a240ae32</t>
+  </si>
+  <si>
     <t>PLSX/WPLS</t>
   </si>
   <si>
+    <t>0x1b45b9148791d3a104184cd5dfe5ce57193a3ee9</t>
+  </si>
+  <si>
+    <t>https://dexscreener.com/pulsechain/0x1b45b9148791d3a104184cd5dfe5ce57193a3ee9</t>
+  </si>
+  <si>
     <t>WPLS/PLSX</t>
   </si>
   <si>
     <t>0x149b2c629e652f2e89e11cd57e5d4d77ee166f9f</t>
+  </si>
+  <si>
+    <t>https://dexscreener.com/pulsechain/0x149b2c629e652f2e89e11cd57e5d4d77ee166f9f</t>
   </si>
 </sst>
 </file>
@@ -131,10 +152,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -148,6 +169,106 @@
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -162,6 +283,20 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -169,121 +304,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -298,187 +319,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -507,20 +528,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -542,10 +560,8 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
+      <top/>
+      <bottom style="medium">
         <color theme="4"/>
       </bottom>
       <diagonal/>
@@ -566,15 +582,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -590,17 +597,31 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
       </top>
       <bottom style="double">
-        <color rgb="FF3F3F3F"/>
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -609,142 +630,142 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="5" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="21" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="23" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1118,13 +1139,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:N6"/>
+  <dimension ref="A1:N7"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="6"/>
   <cols>
     <col min="4" max="4" width="10.5555555555556" customWidth="1"/>
     <col min="5" max="7" width="11.1111111111111" customWidth="1"/>
@@ -1304,10 +1325,14 @@
       <c r="L4" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="M4" s="1"/>
-      <c r="N4" s="4"/>
+      <c r="M4" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="N4" s="4" t="s">
+        <v>34</v>
+      </c>
     </row>
-    <row r="5" ht="30" spans="1:14">
+    <row r="5" ht="75" spans="1:14">
       <c r="A5" s="1" t="s">
         <v>14</v>
       </c>
@@ -1318,34 +1343,38 @@
         <v>15</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>17</v>
+        <v>30</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>31</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>22</v>
+        <v>32</v>
       </c>
       <c r="L5" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="M5" s="1"/>
-      <c r="N5" s="4"/>
+        <v>23</v>
+      </c>
+      <c r="M5" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="N5" s="4" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="6" ht="30" spans="1:14">
       <c r="A6" s="1" t="s">
@@ -1358,41 +1387,91 @@
         <v>15</v>
       </c>
       <c r="D6" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="L6" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="M6" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="N6" s="4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="7" ht="30" spans="1:14">
+      <c r="A7" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E6" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="F6" s="1" t="s">
+      <c r="B7" s="1">
+        <v>369</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F7" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="G6" s="1" t="s">
+      <c r="G7" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="H6" s="2" t="s">
+      <c r="H7" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="I6" s="1" t="s">
+      <c r="I7" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="J6" s="1" t="s">
+      <c r="J7" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="K6" s="1" t="s">
+      <c r="K7" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="L6" s="1" t="s">
+      <c r="L7" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="M6" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="N6" s="4"/>
+      <c r="M7" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="N7" s="4" t="s">
+        <v>42</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="N2" r:id="rId1" display="https://dexscreener.com/pulsechain/0xb2893cea8080bf43b7b60b589edaab5211d98f23" tooltip="https://dexscreener.com/pulsechain/0xb2893cea8080bf43b7b60b589edaab5211d98f23"/>
-    <hyperlink ref="N3" r:id="rId2" display="https://dexscreener.com/pulsechain/0x790c996afe80efe313a9a28ef4221ef5a555b8b2"/>
+    <hyperlink ref="N3" r:id="rId2" display="https://dexscreener.com/pulsechain/0x790c996afe80efe313a9a28ef4221ef5a555b8b2" tooltip="https://dexscreener.com/pulsechain/0x790c996afe80efe313a9a28ef4221ef5a555b8b2"/>
+    <hyperlink ref="N4" r:id="rId3" display="https://dexscreener.com/pulsechain/0xE56043671df55dE5CDf8459710433C10324DE0aE" tooltip="https://dexscreener.com/pulsechain/0xE56043671df55dE5CDf8459710433C10324DE0aE"/>
+    <hyperlink ref="N7" r:id="rId4" display="https://dexscreener.com/pulsechain/0x149b2c629e652f2e89e11cd57e5d4d77ee166f9f"/>
+    <hyperlink ref="N5" r:id="rId5" display="https://dexscreener.com/pulsechain/0x146e1f1e060e5b5016db0d118d2c5a11a240ae32" tooltip="https://dexscreener.com/pulsechain/0x146e1f1e060e5b5016db0d118d2c5a11a240ae32"/>
+    <hyperlink ref="N6" r:id="rId6" display="https://dexscreener.com/pulsechain/0x1b45b9148791d3a104184cd5dfe5ce57193a3ee9"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>

</xml_diff>